<commit_message>
Teste para insertFile( ) : NullPath
</commit_message>
<xml_diff>
--- a/TabelasTestes/ESII Tabelas Testes.xlsx
+++ b/TabelasTestes/ESII Tabelas Testes.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="insertQuery()" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="insertFile()" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>EQUIVALENCE CLASS PARTITIONING insertQuery()</t>
   </si>
   <si>
+    <t>EQUIVALENCE CLASS PARTITIONING insertFile()</t>
+  </si>
+  <si>
     <t>REQUIREMENTS</t>
   </si>
   <si>
@@ -49,7 +53,10 @@
     <t>query: ""</t>
   </si>
   <si>
-    <t>BOUNDARY VALUE ANALYSIS</t>
+    <t>BOUNDARY VALUE ANALYSIS insertQuery()</t>
+  </si>
+  <si>
+    <t>BOUNDARY VALUE ANALYSIS insertFile()</t>
   </si>
   <si>
     <t>LOWER BOUNDRY</t>
@@ -73,6 +80,9 @@
     <t>INVALID PARTITION                  BY ABOVE THE BOUNDRY</t>
   </si>
   <si>
+    <t>filePath</t>
+  </si>
+  <si>
     <t>query</t>
   </si>
   <si>
@@ -88,7 +98,10 @@
     <t>NO MAX AMOUNT</t>
   </si>
   <si>
-    <t>TEST CASES</t>
+    <t>TEST CASES insertFile()</t>
+  </si>
+  <si>
+    <t>TEST CASES insertQuery()</t>
   </si>
   <si>
     <t>TEST CASE ID</t>
@@ -109,13 +122,25 @@
     <t>Test Status</t>
   </si>
   <si>
+    <t>Invalid Path</t>
+  </si>
+  <si>
+    <t>fm (FileManager) being declared</t>
+  </si>
+  <si>
+    <t>Invalid path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False </t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>query inválida</t>
   </si>
   <si>
-    <t xml:space="preserve">False </t>
-  </si>
-  <si>
-    <t>Passed</t>
+    <t>Null path</t>
   </si>
   <si>
     <t>query válida</t>
@@ -125,6 +150,12 @@
   </si>
   <si>
     <t xml:space="preserve">True </t>
+  </si>
+  <si>
+    <t>Valid Path</t>
+  </si>
+  <si>
+    <t>Valid path</t>
   </si>
 </sst>
 </file>
@@ -288,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -318,7 +349,7 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -348,7 +379,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,6 +404,7 @@
     <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -385,6 +417,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -434,13 +470,13 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -451,13 +487,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="8">
         <v>1.0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -468,13 +504,13 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -485,13 +521,13 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -513,59 +549,59 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I10" s="16"/>
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I12" s="20"/>
     </row>
@@ -593,7 +629,7 @@
     </row>
     <row r="15">
       <c r="A15" s="22" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -604,25 +640,25 @@
     </row>
     <row r="16">
       <c r="A16" s="23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -630,7 +666,7 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
@@ -641,22 +677,22 @@
         <v>1.0</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
@@ -664,20 +700,20 @@
         <v>2.0</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="28" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>34</v>
+        <v>45</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -706,4 +742,343 @@
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.86"/>
+    <col customWidth="1" min="2" max="2" width="25.57"/>
+    <col customWidth="1" min="3" max="3" width="31.0"/>
+    <col customWidth="1" min="4" max="4" width="15.14"/>
+    <col customWidth="1" min="5" max="5" width="23.0"/>
+    <col customWidth="1" min="6" max="6" width="23.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A15:G15"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tabelas Testes uniqueWords( )
</commit_message>
<xml_diff>
--- a/TabelasTestes/ESII Tabelas Testes.xlsx
+++ b/TabelasTestes/ESII Tabelas Testes.xlsx
@@ -7,6 +7,10 @@
     <sheet state="visible" name="insertFile()" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="removeDigits()" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="removeChars()" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="uniqueWords" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="matrizOrganizer" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="matrizModifier" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="calculoGrauS" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="70">
   <si>
     <t>EQUIVALENCE CLASS PARTITIONING removeDigits()</t>
   </si>
@@ -22,24 +26,24 @@
     <t>REQUIREMENTS</t>
   </si>
   <si>
+    <t>EQUIVALENCE CLASS PARTITIONING insertQuery()</t>
+  </si>
+  <si>
     <t>VALID CLASS</t>
   </si>
   <si>
+    <t>INVALID CLASS</t>
+  </si>
+  <si>
+    <t>Nº INPUTS</t>
+  </si>
+  <si>
+    <t>!=1</t>
+  </si>
+  <si>
     <t>EQUIVALENCE CLASS PARTITIONING insertFile()</t>
   </si>
   <si>
-    <t>EQUIVALENCE CLASS PARTITIONING insertQuery()</t>
-  </si>
-  <si>
-    <t>INVALID CLASS</t>
-  </si>
-  <si>
-    <t>Nº INPUTS</t>
-  </si>
-  <si>
-    <t>!=1</t>
-  </si>
-  <si>
     <t>INPUT TYPES</t>
   </si>
   <si>
@@ -58,18 +62,18 @@
     <t>query: ""</t>
   </si>
   <si>
+    <t>BOUNDARY VALUE ANALYSIS removeDigits()</t>
+  </si>
+  <si>
     <t>BOUNDARY VALUE ANALYSIS insertQuery()</t>
   </si>
   <si>
+    <t>LOWER BOUNDRY</t>
+  </si>
+  <si>
     <t>BOUNDARY VALUE ANALYSIS insertFile()</t>
   </si>
   <si>
-    <t>BOUNDARY VALUE ANALYSIS removeDigits()</t>
-  </si>
-  <si>
-    <t>LOWER BOUNDRY</t>
-  </si>
-  <si>
     <t>UPPER BOUNDRY</t>
   </si>
   <si>
@@ -88,12 +92,12 @@
     <t>INVALID PARTITION                  BY ABOVE THE BOUNDRY</t>
   </si>
   <si>
+    <t>filePath</t>
+  </si>
+  <si>
     <t>query</t>
   </si>
   <si>
-    <t>filePath</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
@@ -106,15 +110,15 @@
     <t>NO MAX AMOUNT</t>
   </si>
   <si>
+    <t>TEST CASES removeDigits()</t>
+  </si>
+  <si>
+    <t>TEST CASES insertQuery()</t>
+  </si>
+  <si>
     <t>TEST CASES insertFile()</t>
   </si>
   <si>
-    <t>TEST CASES insertQuery()</t>
-  </si>
-  <si>
-    <t>TEST CASES removeDigits()</t>
-  </si>
-  <si>
     <t>TEST CASE ID</t>
   </si>
   <si>
@@ -133,16 +137,28 @@
     <t>Test Status</t>
   </si>
   <si>
+    <t>query inválida</t>
+  </si>
+  <si>
+    <t>fm (FileManager) being declared</t>
+  </si>
+  <si>
+    <t>Invalid Path</t>
+  </si>
+  <si>
+    <t>Invalid path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False </t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>texto</t>
   </si>
   <si>
-    <t>Invalid Path</t>
-  </si>
-  <si>
-    <t>fm (FileManager) being declared</t>
-  </si>
-  <si>
-    <t>query inválida</t>
+    <t>Null path</t>
   </si>
   <si>
     <t>Digits Being Removed</t>
@@ -151,10 +167,13 @@
     <t>fm (FileManager) being declared &amp;&amp; String has numbers</t>
   </si>
   <si>
-    <t xml:space="preserve">False </t>
-  </si>
-  <si>
-    <t>Passed</t>
+    <t>Valid Path</t>
+  </si>
+  <si>
+    <t>Valid path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True </t>
   </si>
   <si>
     <t>texto with Numbers</t>
@@ -169,31 +188,34 @@
     <t>"anything"</t>
   </si>
   <si>
-    <t xml:space="preserve">True </t>
-  </si>
-  <si>
-    <t>Invalid path</t>
-  </si>
-  <si>
-    <t>Null path</t>
-  </si>
-  <si>
-    <t>Valid Path</t>
-  </si>
-  <si>
-    <t>Valid path</t>
-  </si>
-  <si>
     <t>EQUIVALENCE CLASS PARTITIONING removeChars()</t>
   </si>
   <si>
+    <t>EQUIVALENCE CLASS PARTITIONING uniqueWords()</t>
+  </si>
+  <si>
     <t>BOUNDARY VALUE ANALYSIS removeChars()</t>
   </si>
   <si>
+    <t>BOUNDARY VALUE ANALYSIS uniqueWords()</t>
+  </si>
+  <si>
     <t>TEST CASES removeChars()</t>
   </si>
   <si>
+    <t>TEST CASES uniqueWords()</t>
+  </si>
+  <si>
     <t>Special Characters Being Removed</t>
+  </si>
+  <si>
+    <t>Extra words Being Removed</t>
+  </si>
+  <si>
+    <t>texto with duplicated words</t>
+  </si>
+  <si>
+    <t>String With No duplicated words</t>
   </si>
   <si>
     <t>fm (FileManager) being declared &amp;&amp; String has special characters</t>
@@ -424,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -496,46 +518,49 @@
     <xf borderId="7" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="10" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="10" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -557,6 +582,22 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -593,7 +634,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -609,10 +650,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -623,13 +664,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="8">
         <v>1.0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -685,13 +726,13 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>18</v>
@@ -720,7 +761,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>26</v>
@@ -784,7 +825,7 @@
       <c r="C16" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="26" t="s">
@@ -798,58 +839,58 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18">
-      <c r="A18" s="35">
+      <c r="A18" s="34">
         <v>1.0</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="33" t="s">
+      <c r="B18" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="39" t="s">
-        <v>46</v>
+      <c r="E18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="35">
+      <c r="A19" s="34">
         <v>2.0</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="33" t="s">
+      <c r="B19" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="41" t="s">
-        <v>46</v>
+      <c r="G19" s="40" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -857,24 +898,24 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="A15:G15"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -911,7 +952,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -927,10 +968,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -941,13 +982,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="8">
         <v>1.0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1003,13 +1044,13 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>18</v>
@@ -1038,7 +1079,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>26</v>
@@ -1083,7 +1124,7 @@
     </row>
     <row r="15">
       <c r="A15" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1102,7 +1143,7 @@
       <c r="C16" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="26" t="s">
@@ -1116,79 +1157,79 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18">
-      <c r="A18" s="35">
+      <c r="A18" s="34">
         <v>1.0</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="39" t="s">
+      <c r="C19" s="38"/>
+      <c r="D19" s="32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="35">
+      <c r="E19" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="34">
         <v>2.0</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="33" t="s">
+      <c r="B20" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="41" t="s">
-        <v>46</v>
+      <c r="G20" s="40" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1196,24 +1237,24 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="A15:G15"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1257,10 +1298,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1271,13 +1312,13 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="8">
         <v>1.0</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1333,13 +1374,13 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>18</v>
@@ -1368,7 +1409,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>26</v>
@@ -1413,70 +1454,70 @@
     </row>
     <row r="14">
       <c r="A14" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="27"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17">
-      <c r="A17" s="36">
+      <c r="A17" s="39">
         <v>1.0</v>
       </c>
-      <c r="B17" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="38" t="s">
+      <c r="B17" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="42" t="s">
         <v>44</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1488,19 +1529,19 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A14:G14"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="F8:I8"/>
+    <mergeCell ref="I9:I10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="A7:I7"/>
-    <mergeCell ref="I9:I10"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1542,10 +1583,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1556,13 +1597,13 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="8">
         <v>1.0</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1618,13 +1659,13 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>18</v>
@@ -1653,7 +1694,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>26</v>
@@ -1698,70 +1739,70 @@
     </row>
     <row r="14">
       <c r="A14" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="27"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="36">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" ht="47.25" customHeight="1">
+      <c r="A17" s="39">
         <v>1.0</v>
       </c>
-      <c r="B17" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="34" t="s">
+      <c r="B17" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>46</v>
+      <c r="C17" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1789,4 +1830,330 @@
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.57"/>
+    <col customWidth="1" min="2" max="2" width="28.43"/>
+    <col customWidth="1" min="3" max="3" width="26.14"/>
+    <col customWidth="1" min="4" max="5" width="19.14"/>
+    <col customWidth="1" min="6" max="6" width="19.86"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" ht="42.0" customHeight="1">
+      <c r="A18" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="H10:H11"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>